<commit_message>
Start and End Time
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataManageListings.xlsx
+++ b/MarsFramework/ExcelData/TestDataManageListings.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0956pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1144pm</t>
   </si>
   <si>
     <t xml:space="preserve">Performance Testing</t>
@@ -145,11 +151,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="hh:mm:ss;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -241,7 +246,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,10 +272,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -358,7 +359,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
@@ -426,7 +427,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -478,15 +479,15 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.43"/>
@@ -577,17 +578,17 @@
       <c r="J2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="7" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="L2" s="7" t="n">
-        <v>0.833333333333333</v>
+      <c r="K2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O2" s="3" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
updated nuget packages, chromedriver and config parameters
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataManageListings.xlsx
+++ b/MarsFramework/ExcelData/TestDataManageListings.xlsx
@@ -129,10 +129,10 @@
     <t xml:space="preserve">Online</t>
   </si>
   <si>
-    <t xml:space="preserve">12012022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20052022</t>
+    <t xml:space="preserve">12092022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20092022</t>
   </si>
   <si>
     <t xml:space="preserve">Tue</t>
@@ -360,7 +360,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
@@ -428,7 +428,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -480,11 +480,11 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.29"/>

</xml_diff>